<commit_message>
working on the analysis
</commit_message>
<xml_diff>
--- a/test_utf8.xlsx
+++ b/test_utf8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/big_team_who/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D77A340-C039-CA44-8402-81C7295614C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E825437-68F7-FA45-8B33-90D7B57EC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C44F954D-A887-784F-B316-8415FCA70218}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13734" uniqueCount="5062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13735" uniqueCount="5063">
   <si>
     <t>last</t>
   </si>
@@ -15221,6 +15221,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>ReD-s38AAAAJ</t>
   </si>
 </sst>
 </file>
@@ -15610,8 +15613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281DB976-6238-4E4A-B6E3-3ED7B1F831C6}">
   <dimension ref="A1:G3371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A2927" workbookViewId="0">
+      <selection activeCell="F2948" sqref="F2948"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57495,7 +57498,7 @@
         <v>4389</v>
       </c>
     </row>
-    <row r="2945" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2945" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2945" s="2" t="s">
         <v>535</v>
       </c>
@@ -57509,7 +57512,7 @@
         <v>4389</v>
       </c>
     </row>
-    <row r="2946" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2946" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2946" s="2" t="s">
         <v>545</v>
       </c>
@@ -57526,7 +57529,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="2947" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2947" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2947" s="2" t="s">
         <v>645</v>
       </c>
@@ -57543,7 +57546,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="2948" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2948" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2948" s="2" t="s">
         <v>1812</v>
       </c>
@@ -57560,7 +57563,7 @@
         <v>1813</v>
       </c>
     </row>
-    <row r="2949" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2949" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2949" s="2" t="s">
         <v>964</v>
       </c>
@@ -57576,8 +57579,11 @@
       <c r="E2949" s="2" t="s">
         <v>1818</v>
       </c>
-    </row>
-    <row r="2950" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2949" s="2" t="s">
+        <v>5062</v>
+      </c>
+    </row>
+    <row r="2950" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2950" s="2" t="s">
         <v>1809</v>
       </c>
@@ -57594,7 +57600,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="2951" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2951" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2951" s="2" t="s">
         <v>491</v>
       </c>
@@ -57608,7 +57614,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2952" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2952" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2952" s="2" t="s">
         <v>1804</v>
       </c>
@@ -57622,7 +57628,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2953" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2953" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2953" s="2" t="s">
         <v>1103</v>
       </c>
@@ -57636,7 +57642,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2954" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2954" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2954" s="2" t="s">
         <v>22</v>
       </c>
@@ -57650,7 +57656,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2955" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2955" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2955" s="2" t="s">
         <v>1816</v>
       </c>
@@ -57664,7 +57670,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2956" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2956" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2956" s="2" t="s">
         <v>4448</v>
       </c>
@@ -57681,7 +57687,7 @@
         <v>4449</v>
       </c>
     </row>
-    <row r="2957" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2957" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2957" s="2" t="s">
         <v>4430</v>
       </c>
@@ -57695,7 +57701,7 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="2958" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2958" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2958" s="2" t="s">
         <v>4442</v>
       </c>
@@ -57709,7 +57715,7 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="2959" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2959" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2959" s="2" t="s">
         <v>4464</v>
       </c>
@@ -57723,7 +57729,7 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="2960" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2960" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2960" s="2" t="s">
         <v>623</v>
       </c>

</xml_diff>